<commit_message>
Added test for stability status for the ShellSort
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Compumar\Documents\Projects\npadros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Compumar\Documents\Project\npadros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,11 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="27" formatCode="d/m/yyyy\ hh:mm"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -677,7 +681,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistics!$K$8</c:f>
+              <c:f>Statistics!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -779,7 +783,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Statistics!$M$8:$P$8</c:f>
+              <c:f>Statistics!$D$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -809,7 +813,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistics!$K$9</c:f>
+              <c:f>Statistics!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -911,7 +915,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Statistics!$M$9:$P$9</c:f>
+              <c:f>Statistics!$D$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1225,7 +1229,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistics!$K$10</c:f>
+              <c:f>Statistics!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1327,7 +1331,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Statistics!$M$10:$P$10</c:f>
+              <c:f>Statistics!$D$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1357,7 +1361,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistics!$K$11</c:f>
+              <c:f>Statistics!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1459,7 +1463,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Statistics!$M$11:$P$11</c:f>
+              <c:f>Statistics!$D$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1768,7 +1772,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistics!$B$2</c:f>
+              <c:f>Statistics!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1870,7 +1874,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Statistics!$D$2:$G$2</c:f>
+              <c:f>Statistics!$D$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1900,7 +1904,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistics!$B$3</c:f>
+              <c:f>Statistics!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2002,7 +2006,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Statistics!$D$3:$G$3</c:f>
+              <c:f>Statistics!$D$7:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4170,6 +4174,22 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:G7" totalsRowShown="0">
+  <autoFilter ref="A1:G7"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="DATE" dataDxfId="0"/>
+    <tableColumn id="2" name="SEQUENCE ORDER"/>
+    <tableColumn id="3" name="DATA TYPE"/>
+    <tableColumn id="4" name="LENGTH"/>
+    <tableColumn id="5" name="SWAPS"/>
+    <tableColumn id="6" name="COMPARITIONS"/>
+    <tableColumn id="7" name="NANO TIME"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -4467,19 +4487,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="B1:B3 D1:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4502,9 +4526,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42612.378391203703</v>
+        <v>42612.37767361111</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -4513,21 +4537,21 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>24502102</v>
+        <v>2558</v>
       </c>
       <c r="F2">
-        <v>24566443</v>
+        <v>2845</v>
       </c>
       <c r="G2">
-        <v>175198</v>
+        <v>10572</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42612.378391203703</v>
+        <v>42612.37767361111</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -4536,112 +4560,115 @@
         <v>6</v>
       </c>
       <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>2558</v>
+      </c>
+      <c r="F3">
+        <v>3187</v>
+      </c>
+      <c r="G3">
+        <v>11705</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42612.378321759257</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>247685</v>
+      </c>
+      <c r="F4">
+        <v>252286</v>
+      </c>
+      <c r="G4">
+        <v>27186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42612.378321759257</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <v>247685</v>
+      </c>
+      <c r="F5">
+        <v>257743</v>
+      </c>
+      <c r="G5">
+        <v>26809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42612.378391203703</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
         <v>10000</v>
       </c>
-      <c r="E3">
+      <c r="E6">
         <v>24502102</v>
       </c>
-      <c r="F3">
+      <c r="F6">
+        <v>24566443</v>
+      </c>
+      <c r="G6">
+        <v>175198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42612.378391203703</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>10000</v>
+      </c>
+      <c r="E7">
+        <v>24502102</v>
+      </c>
+      <c r="F7">
         <v>24641686</v>
       </c>
-      <c r="G3">
+      <c r="G7">
         <v>6796</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J8" s="1">
-        <v>42612.37767361111</v>
-      </c>
-      <c r="K8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8">
-        <v>100</v>
-      </c>
-      <c r="N8">
-        <v>2558</v>
-      </c>
-      <c r="O8">
-        <v>2845</v>
-      </c>
-      <c r="P8">
-        <v>10572</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J9" s="1">
-        <v>42612.37767361111</v>
-      </c>
-      <c r="K9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M9">
-        <v>100</v>
-      </c>
-      <c r="N9">
-        <v>2558</v>
-      </c>
-      <c r="O9">
-        <v>3187</v>
-      </c>
-      <c r="P9">
-        <v>11705</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J10" s="1">
-        <v>42612.378321759257</v>
-      </c>
-      <c r="K10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L10" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10">
-        <v>1000</v>
-      </c>
-      <c r="N10">
-        <v>247685</v>
-      </c>
-      <c r="O10">
-        <v>252286</v>
-      </c>
-      <c r="P10">
-        <v>27186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J11" s="1">
-        <v>42612.378321759257</v>
-      </c>
-      <c r="K11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11">
-        <v>1000</v>
-      </c>
-      <c r="N11">
-        <v>247685</v>
-      </c>
-      <c r="O11">
-        <v>257743</v>
-      </c>
-      <c r="P11">
-        <v>26809</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4649,7 +4676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>